<commit_message>
updates for prior with sigma
</commit_message>
<xml_diff>
--- a/variable_summary.xlsx
+++ b/variable_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lgorman/research/phd/chapter-6-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54034175-9132-224A-961D-6578AB7E5C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B94D393-B6F4-A041-80EC-02004FC49A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="variable_summary" sheetId="1" r:id="rId1"/>
@@ -411,14 +411,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Bell MT"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Bell MT"/>
       <family val="1"/>
@@ -605,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -805,6 +805,26 @@
       <right/>
       <top style="medium">
         <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2" tint="-0.499984740745262"/>
       </top>
       <bottom style="thin">
         <color theme="2" tint="-0.499984740745262"/>
@@ -856,93 +876,102 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1300,91 +1329,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I22"/>
+  <dimension ref="B1:I26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" style="2" customWidth="1"/>
-    <col min="7" max="7" width="28" style="28" customWidth="1"/>
-    <col min="8" max="8" width="13" style="28" customWidth="1"/>
-    <col min="9" max="9" width="34.6640625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="20.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="28" style="3" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="61.6640625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+    <row r="1" spans="2:9" ht="25" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:9" ht="25" x14ac:dyDescent="0.2">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B4" s="7"/>
-      <c r="C4" s="26" t="s">
+    <row r="4" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B4" s="8"/>
+      <c r="C4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="16" t="s">
         <v>56</v>
       </c>
       <c r="G4" s="17" t="s">
@@ -1393,22 +1422,22 @@
       <c r="H4" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B5" s="7"/>
-      <c r="C5" s="26" t="s">
+    <row r="5" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B5" s="8"/>
+      <c r="C5" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="16" t="s">
         <v>59</v>
       </c>
       <c r="G5" s="17" t="s">
@@ -1417,427 +1446,430 @@
       <c r="H5" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="27" t="s">
+    <row r="6" spans="2:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="27" t="s">
+      <c r="G6" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="25" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="102" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
+    <row r="7" spans="2:9" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="11" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
-      <c r="C8" s="27" t="s">
+    <row r="8" spans="2:9" ht="51" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-      <c r="C10" s="27" t="s">
+    <row r="10" spans="2:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="19"/>
+      <c r="C10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="25" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+    <row r="11" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="26" t="s">
+    <row r="12" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B12" s="8"/>
+      <c r="C12" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="7"/>
-      <c r="C13" s="26" t="s">
+      <c r="I12" s="16"/>
+    </row>
+    <row r="13" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B13" s="8"/>
+      <c r="C13" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="16" t="s">
         <v>47</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="16" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="26" t="s">
+    <row r="14" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B14" s="8"/>
+      <c r="C14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="F14" s="16" t="s">
         <v>48</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="16" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="8"/>
-      <c r="C15" s="27" t="s">
+    <row r="15" spans="2:9" ht="51" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="19"/>
+      <c r="C15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="25" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B16" s="7" t="s">
+    <row r="16" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="11" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
-      <c r="C17" s="26" t="s">
+    <row r="17" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B17" s="8"/>
+      <c r="C17" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F17" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="G17" s="29" t="s">
         <v>79</v>
       </c>
       <c r="H17" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="2:9" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="8"/>
-      <c r="C18" s="27" t="s">
+    <row r="18" spans="2:9" ht="51" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="F18" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="25" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="2:9" ht="50" x14ac:dyDescent="0.2">
+      <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G19" s="16" t="s">
+      <c r="G19" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="H19" s="16" t="s">
+      <c r="H19" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="11" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="8"/>
-      <c r="C20" s="27" t="s">
+    <row r="20" spans="2:9" ht="76" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="25" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
+    <row r="21" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="H21" s="16" t="s">
+      <c r="H21" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="8"/>
-      <c r="C22" s="27" t="s">
+    <row r="22" spans="2:9" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="I22" s="18" t="s">
+      <c r="I22" s="24" t="s">
         <v>78</v>
       </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="F26" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>